<commit_message>
PCOS class scraping data with eliminators
</commit_message>
<xml_diff>
--- a/src/test/resources/outPutData.xlsx
+++ b/src/test/resources/outPutData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayesh\IdeaProjects\Data_Scraping_Framework_Demo1\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CB4DAF-1142-4DA1-A5C3-8BFDBDF49302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D30959-7816-4211-8786-2E37860A71D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PCOS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,35 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>A Checkerboard Of Roses ( Flower Arrangements)</t>
-  </si>
-  <si>
-    <t>A Truly Delectable Bunch ( Flower Arrangements)</t>
-  </si>
-  <si>
-    <t>A-bun-dantly Creative ( Flower Arrangements)</t>
-  </si>
-  <si>
-    <t>aam chana achar recipe | Rajasthani aam chana ka achar | Indian mango pickle with chana | kabuli chana achar |</t>
-  </si>
-  <si>
-    <t>aam ka achar recipe | Punjabi aam ka achar | mango pickle |</t>
-  </si>
-  <si>
-    <t>Aam Ke Pakode, Mango Bhajiya</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Aam ki Katki ka Muraba</t>
+  </si>
+  <si>
+    <t>Recipe Name</t>
+  </si>
+  <si>
+    <t>Recipe Category(Breakfast/lunch/snack/dinner)</t>
+  </si>
+  <si>
+    <t>Food Category(Veg/non-veg/vegan/Jain)</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Preparation Time</t>
+  </si>
+  <si>
+    <t>Cooking Time</t>
+  </si>
+  <si>
+    <t>Preparation method</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,16 +63,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,15 +97,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{72C4CCDD-48E5-4AE9-931F-412CBC6391DF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -364,17 +403,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="2">
+    <row r="1" spans="1:10" ht="75">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed scraping of recipes for one page and writing the data to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/outPutData.xlsx
+++ b/src/test/resources/outPutData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayesh\IdeaProjects\Data_Scraping_Framework_Demo1\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D30959-7816-4211-8786-2E37860A71D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1605FC-DC0B-44AB-8B0D-04A9214EED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,36 +25,573 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+  <si>
+    <t>Recipe Name</t>
+  </si>
+  <si>
+    <t>Recipe Category(Breakfast/lunch/snack/dinner)</t>
+  </si>
+  <si>
+    <t>Food Category(Veg/non-veg/vegan/Jain)</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Preparation Time</t>
+  </si>
+  <si>
+    <t>Cooking Time</t>
+  </si>
+  <si>
+    <t>Preparation method</t>
+  </si>
+  <si>
+    <t>RecipeId</t>
+  </si>
+  <si>
+    <t>Nutrient Value</t>
+  </si>
+  <si>
+    <t>recipeUrl</t>
+  </si>
+  <si>
+    <t>A Checkerboard Of Roses ( Flower Arrangements)</t>
+  </si>
+  <si>
+    <t>No Cooking Veg Indian</t>
+  </si>
+  <si>
+    <t>Thing You Will Need
+a square , flat tray , or a sheet of stone floral foam
+green asparagus of good quality and uniform appearance
+lemongrass
+roses of similar sizes and colours to match your decor
+asparagus ferns ( plumosis)</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>0 mins</t>
+  </si>
+  <si>
+    <t>Method
+Soak the piece of foam well in water before placing it on the tray. Keep the tray at the place where you want to set up the arrangement. Slice the foam to a very low height, in keeping with the height of your low dining-table sit-down.
+Depending on their thickness, make four equal-looking bundles of the asparagus, probably using 8 to 10 stems in each. Tie each bundle up with lemongrass and place the bundles along the base of the tray, forming a square. Then tie the four corners with lemongrass to hold the asparagus in place.
+Before using the roses, cut the stems to about 6" to 8" and leave them in water for about 1/2 hour so that they last longer. Here we have chosen pink and white roses.
+Place the roses first in the outer square of the sponge, alternating the white with the pink. Then, in a similar manner, fill up the whole square.
+To finish off, use the asparagus ferns to cover up any spaces where the foam is still visible.
+Handy tip
+If you find asparagus difficult to find, use small drumsticks instead.</t>
+  </si>
+  <si>
+    <t>A Truly Delectable Bunch ( Flower Arrangements)</t>
+  </si>
+  <si>
+    <t>You Will Need
+eclairs/ toffees available in the market
+filler greens
+roses
+kebab sticks
+white thread
+green tape
+basket with moss fixed in it</t>
+  </si>
+  <si>
+    <t>Method
+Take a long kebab stick and tie one of the éclairs on top with the white thread.
+Make a loop with the thread and tie it securely to the stick.
+Take the second éclair and tie it at right angles to the first one.
+Tie the third éclair opposite the second one.
+Continue in the same way till you have tied a lot of éclairs on the stick.
+Wrap the rest of the kebab stick with green tape.
+Make many more sticks in the same way.
+Lay out the basket, roses and the éclair sticks. Use small fillers made of chocolate wrapped in cellophane and tied to toothpicks.
+Stick all the green fillers into the moss and then start adding the roses one by one.
+Now place the éclair sticks in between the roses and fillers.
+Arrange the éclair sticks in such a way that the bouquet looks balanced.
+Fill the gaps with the small chocolate fillers.
+Your delicious chocolate bouquet is ready!</t>
+  </si>
+  <si>
+    <t>A-bun-dantly Creative ( Flower Arrangements)</t>
+  </si>
+  <si>
+    <t>Thing You Will Need
+5 roll buns
+4 gerberas ( of the same colour)
+a few asparagus ferns
+a cane mat (10" by 6")
+scissors
+2 round block candles ( preferably green in colour)
+a few wedges of lavash
+2 pieces of raffia , refer handy tip</t>
+  </si>
+  <si>
+    <t>Method
+Start by placing a protective covering over your table. Place a cane mat in the center of the table. Take 5 roll buns and place them horizontally on a mat at an equal distance form each other.
+Place a gerbera between 2 roll buns in a raised position as shown in the picture.
+Add some asparagus ferns to add colour. They can be placed beneath the petals.
+Cut the lavash bread into triangles of various sizes. Use raffia to tie the triangles around a round candle. Decorate 2 candles in this manner. Place the candles on oppsite corners of the mat near the bread.
+Your eye-catching centerpiece is ready.
+Handy tip
+Raffia is a soft natural fibre sued for weaving, winding and making baskets, mats and many other items.</t>
+  </si>
+  <si>
+    <t>aam chana achar recipe | Rajasthani aam chana ka achar | Indian mango pickle with chana | kabuli chana achar |</t>
+  </si>
+  <si>
+    <t>For Aam Chana Achar
+1 1/2 cups grated raw mango
+1/2 cup kabuli chana (white chick peas)
+1 tsp turmeric powder (haldi)
+salt to taste
+1 tbsp fenugreek (methi) seeds
+1 tbsp fenugreek seeds (methi) powder
+1 tbsp fennel seeds (saunf)
+1/2 tsp asafoetida (hing)
+1 tsp nigella seeds (kalonji)
+7 whole dry kashmiri red chillies
+1 tbsp chilli powder
+1 1/4 cups mustard (rai / sarson) oil</t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>4 mins</t>
+  </si>
+  <si>
+    <t>Method
+For aam chana achar
+To make aam chana achar, combine the raw mango, turmeric powder and salt in a deep bowl, mix well and keep aside for 30 minutes.
+Squeeze out all the water from the raw mango in a bowl and keep aside. Keep the raw mango water and grated raw mango separately.
+Refrigerate the grated raw mango overnight.
+Combine the fenugreek seeds, kabuli chana and raw mango water into a deep bowl, mix well and cover and keep aside overnight.
+Combine the fenugreek seed powder, fennel seeds, asafoetida, nigella seeds, kashmiri red chillies, chilli powder along the grated raw mango and kabuli chana-fenugreek seeds mixture into a deep bowl, mix well and keep aside.
+Heat the mustard oil in a deep non-stick kadhai on a medium flame for 3 to 4 minutes or till red hot.
+Remove from the flame and allow it to cool.
+Once cooled, add the oil to the prepared mixture and mix well.
+Bottle the pickle in a sterilized glass jar and keep aside for 6 to 7 days. After 7 days, it is ready to eat.</t>
+  </si>
+  <si>
+    <t>Energy 95 cal
+Protein 0.5 g
+Carbohydrates 3 g
+Fiber 1 g
+Fat 9.1 g
+Cholesterol 0 mg
+Sodium 0.8 mg</t>
+  </si>
+  <si>
+    <t>aam ka achar recipe | Punjabi aam ka achar | mango pickle |</t>
+  </si>
+  <si>
+    <t>For Aam ka Achaar
+5 cups raw mangoes , cut into pieces
+1 tsp turmeric powder (haldi)
+1/4 cup fennel seeds (saunf) , coarsely ground
+1 tbsp split fenugreek seeds (methi na kuria)
+2 tbsp split mustard seeds (rai na kuria)
+1/2 tsp nigella seeds (kalonji)
+1/4 tsp asafoetida (hing)
+2 tbsp chilli powder
+3/4 cup mustard (rai / sarson) oil
+4 tbsp salt</t>
+  </si>
+  <si>
+    <t>15 mins</t>
+  </si>
+  <si>
+    <t>Method
+For aam ka achaar
+To make aam ka achaar, combine the mangoes, turmeric powder and 2 tbsp of salt and toss well.
+Place the mangoes on a sieve, cover with a muslin cloth and place under the sun for 4 to 6 hours.
+Combine the rest of the ingredients in a bowl and mix well.
+Add the mangoes and toss well.
+Bottle the pickle in a sterilised glass jar. Place the pickle under the sun for 4 to 5 days. This aam ka achaar can be stored for upto 1 year.</t>
+  </si>
+  <si>
+    <t>Energy 507 cal
+Protein 1.9 g
+Carbohydrates 62 g
+Fiber 6.6 g
+Fat 31.1 g
+Cholesterol 0 mg
+Sodium 6208.7 mg</t>
+  </si>
+  <si>
+    <t>Aam Ke Pakode, Mango Bhajiya</t>
+  </si>
+  <si>
+    <t>1 1/2 cups riped alphonso mango cubes
+oil for deep-frying
+To Be Mixed Into A Thick Batter (using Approx. 3/4 Cup Of Water)
+3/4 cup besan (bengal gram flour)
+1/4 cup rice flour (chawal ka atta)
+1/4 tsp carom seeds (ajwain)
+1/2 tsp chilli powder
+1/4 tsp turmeric powder (haldi)
+2 pinches asafoetida (hing)
+salt to taste</t>
+  </si>
+  <si>
+    <t>20 mins</t>
+  </si>
+  <si>
+    <t>Method
+Heat the oil in a deep non-stick pan, dip the mango cubes individually into the batter and deep-fry till they turn golden brown and crisp from all the sides. Drain on an absorbent paper.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 237 cal
+Protein 5.8 g
+Carbohydrates 27.3 g
+Fiber 4.2 g
+Fat 11.6 g
+Cholesterol 0 mg
+Vitamin A 1273.8 mcg
+Vitamin B1 0.2 mg
+Vitamin B2 0.1 mg
+Vitamin B3 1.1 mg
+Vitamin C 7 mg
+Folic Acid 36.6 mcg
+Calcium 20.3 mg
+Iron 1.9 mg
+Magnesium 0 mg
+Phosphorus 0 mg
+Sodium 28.9 mg
+Potassium 268.4 mg
+Zinc 0.6 mg</t>
+  </si>
   <si>
     <t>Aam ki Katki ka Muraba</t>
   </si>
   <si>
-    <t>Recipe Name</t>
-  </si>
-  <si>
-    <t>Recipe Category(Breakfast/lunch/snack/dinner)</t>
-  </si>
-  <si>
-    <t>Food Category(Veg/non-veg/vegan/Jain)</t>
-  </si>
-  <si>
-    <t>Ingredients</t>
-  </si>
-  <si>
-    <t>Preparation Time</t>
-  </si>
-  <si>
-    <t>Cooking Time</t>
-  </si>
-  <si>
-    <t>Preparation method</t>
+    <t>2 cups finely chopped raw mango
+1/4 cup grated raw mango
+2 cups (400 grams) sugar
+2 tbsp Sambhaar
+2 tbsp peeled and sliced almonds
+1 tsp poppy seeds (khus-khus)
+1/2 tsp salt</t>
+  </si>
+  <si>
+    <t>15 mins.</t>
+  </si>
+  <si>
+    <t>45 mins.</t>
+  </si>
+  <si>
+    <t>Method
+Combine the sugar with 3 cups of water and cook till the sugar has dissolved, stirring occasionally.
+Add the mango pieces and grated mangoes and cook over a slow flame (approximately 25 to 30 minutes), stirring occasionally till the sugar syrup is of one string consistency and the mango pieces are soft and translucent.
+Add the sambhaar, almonds, poppy seeds and salt and mix well.
+Allow to cool completely. Bottle in a sterilised glass jar. This can be stored for upto 1 year refrigerated.</t>
+  </si>
+  <si>
+    <t>Energy 69 cal
+Protein 0.3 g
+Carbohydrates 15.2 g
+Fiber 0.1 g
+Fat 0.8 g
+Cholesterol 0 mg
+Sodium 85.7 mg</t>
+  </si>
+  <si>
+    <t>Aam ki Launji</t>
+  </si>
+  <si>
+    <t>1 cup peeled raw mango cubes
+2 tbsp oil
+1/2 tsp fennel seeds (saunf)
+1/4 tsp nigella seeds (kalonji)
+1 tbsp coriander (dhania) powder
+1 tsp chilli powder
+1/4 tsp turmeric powder (haldi)
+1/4 cup sugar
+salt to taste</t>
+  </si>
+  <si>
+    <t>5 mins</t>
+  </si>
+  <si>
+    <t>6 mins</t>
+  </si>
+  <si>
+    <t>Method
+Heat the oil in a broad non-stick pan, add the fennel seeds and nigella seeds and sauté on a medium flame for a few seconds.
+Add the raw mango cubes, mix well and cook on a medium flame for 2 minutes, while stirring continuously.
+Add ¼ cup of water, coriander powder, chilli powder, turmeric powder, sugar and salt,mix well and cook on a medium flame for 2 to 3 minutes, while stirring occasionally.
+Allow the launji to cool completely.
+Once cooled, serve or store in an air-tight container and refrigerate.</t>
+  </si>
+  <si>
+    <t>Energy 56 cal
+Protein 0.1 g
+Carbohydrates 7.5 g
+Fiber 0.3 g
+Fat 3.1 g
+Cholesterol 0 mg
+Sodium 0.3 mg</t>
+  </si>
+  <si>
+    <t>Aam Lassi Slush</t>
+  </si>
+  <si>
+    <t>1 cup alphonso mango cubes
+1 cup curds (dahi)
+1 tbsp chopped mint leaves (phudina)
+4 tbsp sugar
+4 to 5 ice-cubes
+For The Garnish
+a few mint leaves (phudina)</t>
+  </si>
+  <si>
+    <t>Method
+Combine all the ingredients in a mixer and blend till smooth.
+Pour the mixture into a shallow aluminium container and cover it with an aluminium foil.
+Freeze it for approx. 4 to 6 hours or until it is firm.
+Remove it from the freezer and keep aside for 4 to 5 minutes.
+Scrape it with a fork and serve immediately in small glasses garnished with mint leaves.</t>
+  </si>
+  <si>
+    <t>Energy 149 cal
+Protein 2.4 g
+Carbohydrates 24.4 g
+Fiber 0.3 g
+Fat 3.4 g
+Cholesterol 8 mg
+Sodium 18.6 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apple beet carrot juice recipe | abc Indian juice | healthy carrot, beet, apple, ginger drink | </t>
+  </si>
+  <si>
+    <t>For Apple Beet Carrot Juice
+1 1/2 cups carrot cubes
+3/4 cup beetroot cubes
+1/2 cup apple cubes
+1/2 tsp chopped ginger (adrak)
+1 tsp lemon juice
+1 cup water
+15 ice cubes</t>
+  </si>
+  <si>
+    <t>Method
+Juicer method for apple beet carrot juice
+In a high quality blender, put carrot cubes, beetroot cubes, apple cubes , chopped ginger, lemon juice, 1 cup water, 15 ice cubes.
+Blend till smooth.
+Serve apple, beetroot and carrot juice.
+Hopper method for apple beet carrot juice
+Add the carrot cubes, beetroot cubes, apple cubes a few at a time along with chopped ginger (adrak) and lemon juice in the hopper.
+Add some crushed ice in 2 individual glasses and pour equal quantities of the juice over it.
+Serve apple, beetroot and carrot juice immediately.
+Handy tip:
+This recipe makes use of unpeeled fruits and vegetables, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.</t>
+  </si>
+  <si>
+    <t>Energy 34 cal
+Protein 0.8 g
+Carbohydrates 7.3 g
+Fiber 2.6 g
+Fat 0.2 g
+Cholesterol 0 mg
+Sodium 30.7 mg</t>
+  </si>
+  <si>
+    <t>Achaari Aloo Roll ( Wraps and Rolls)</t>
+  </si>
+  <si>
+    <t>For The Aam Aur Chane ka Achaar
+1 1/2 cups grated raw mangoes
+1 tsp turmeric powder (haldi)
+1 tbsp salt
+1 tbsp fenugreek (methi) seeds
+1/2 cup kabuli chana (white chick peas)
+1 tbsp fenugreek seeds (methi) powder
+1 tbsp fennel seeds (saunf)
+1/2 tsp asafoetida (hing)
+1 tsp nigella seeds (kalonji)
+14 whole dry kashmiri red chillies
+1 tbsp chilli powder
+1 1/4 cups mustard (rai / sarson) oil
+For The Spicy Potato Filling
+2 tbsp oil
+1 tsp cumin seeds (jeera)
+1/2 cup finely chopped onions
+2 tsp finely chopped green chillies
+1 tsp grated ginger (adrak)
+1 1/2 cups boiled , peeled and mashed potatoes
+1/2 cup boiled green peas
+2 tsp chaat masala
+2 tsp garam masala
+1 tbsp finely chopped coriander (dhania)
+salt to taste
+Other Ingredients
+1 cup onion rings
+chaat masala to taste
+4 rotis</t>
+  </si>
+  <si>
+    <t>Method
+For aam aur chane ka achaar
+Combine the mangoes, turmeric powder and salt in a bowl, mix well and leave aside for 30 minutes. Squeeze out all the water from the mangoes and keep refrigerated till use.
+Soak the kabuli chana and fenugreek seeds in the mango water overnight.
+Combine the fenugreek seeds powder, fennel seeds, asafoetida, nigella seeds, whole red chillies, chilli powder, soaked kabuli chana mixture and grated mangoes in a bowl and mix well.
+Heat the mustard oil in a small pan and cool completely. Add it to the prepared mixture.
+Place the pickle in a sterilised glass jar and store it in a cool dry place.
+The pickle is ready to eat after 3 to 4 days. Store it a cool dry place for upto 1 year.
+For the spicy potato filling
+Heat the oil in a broad pan and add the cumin seeds.
+When the seeds crackle, add the onions and sauté on a medium flame till they turn translucent.
+Add the green chillies and ginger and sauté on a medium flame for 30 seconds.
+Add the potatoes, green peas, chaat masala, garam masala, coriander and salt, mix well and sauté on a medium flame for another 2 to 3 minutes. Keep aside.
+How to proceed
+Combine the onion rings and chaat masala in a bowl, mix well and keep aside.
+Place a roti on a clean dry surface and arrange ¼th of the spicy potato filling in a row in the centre of the roti.
+Spread 1 tsp of aam aur chane ka achaar and arrange ¼ cup of onion rings over it and roll it up tightly.
+Repeat with the remaining ingredients to make 3 more rolls.
+Wrap a tissue paper around each roll and serve immediately.</t>
+  </si>
+  <si>
+    <t>Indian achari paneer tikka recipe | Punjabi style achari paneer tikka | paneer tikka snack | healthy achari tikka |</t>
+  </si>
+  <si>
+    <t>For The Achaari Marinade
+1 tbsp green chilli pickle
+1/2 cup hung curds (chakka dahi)
+1 tsp chopped garlic (lehsun)
+1 tsp fennel seeds (saunf)
+1/2 tsp mustard seeds ( rai / sarson)
+1/4 tsp fenugreek (methi) seeds
+1/4 tsp nigella seeds (kalonji)
+1 tsp cumin seeds (jeera)
+1/4 tsp turmeric powder (haldi)
+1 tbsp mustard (rai / sarson) oil
+salt to taste
+Other Ingredients
+1 1/2 cups paneer (cottage cheese) cubes
+oil for greasing and cooking
+For Serving
+dahiwali pudina chutney</t>
+  </si>
+  <si>
+    <t>Method
+For the achaari marinade
+Combine all the ingredients, except the curds in a mixer and blend to a coarse mixture.
+Transfer the mixture into a deep bowl, add the curds and mix well.
+How to proceed
+To make achaari paneer tikka, add the paneer to the prepared achaari marinade, mix gently and keep aside to marinate for 20 minutes.
+Arrange the marinated paneer cubes equally on satay sticks and keep aside.
+Heat a non-stick tava (griddle), grease it with little oil, place a few satays on it and cook on a medium flame, using a little oil, till they turn golden brown in colour from all the sides.
+Repeat step 3 to cook more satays.
+Serve the achaari paneer tikka immediately with dahiwali phudina chutney.</t>
+  </si>
+  <si>
+    <t>Energy 274 cal
+Protein 9.5 g
+Carbohydrates 7 g
+Fiber 0 g
+Fat 21.9 g
+Cholesterol 8 mg
+Sodium 9.6 mg</t>
+  </si>
+  <si>
+    <t>Achaari Paneer Warqi</t>
+  </si>
+  <si>
+    <t>For The Achaari Paneer
+1 1/2 cups crumbled paneer (cottage cheese)
+2 tbsp mustard (rai / sarson) oil
+2 tsp cumin seeds (jeera)
+1 tsp fennel seeds (saunf)
+1/4 tsp fenugreek (methi) seeds
+1/4 tsp nigella seeds (kalonji)
+1/4 tsp mustard seeds ( rai / sarson)
+1/2 cup finely chopped onions
+2 tsp grated ginger (adrak)
+1 tsp finely chopped green chillies
+1/4 tsp turmeric powder (haldi)
+1/4 cup chopped coriander (dhania)
+salt to taste
+For The Warqi
+5 samosa pattis
+a pinch nigella seeds (kalonji)
+a pinch turmeric powder (haldi)
+a pinch chilli powder
+1 tbsp oil</t>
+  </si>
+  <si>
+    <t>Method
+For the achaari paneer
+Heat the oil in a pan and add the cumin seeds, fenugreek seeds, fennel seeds, onion seeds and mustard seeds.
+When the seeds crackle, add the onions, green chillies, ginger, garlic and sauté for 2 minutes.
+Add the paneer, turmeric powder, coriander and salt and mix well, cook for 3-4 minutes.
+Keep aside.
+For the warqi
+Arrange the samosa pattis one on top of other on a baking tray, using oil to grease between the sheets. Sprinkle with onion seeds, turmeric powder and chilli powder.
+Bake in a pre-heated oven at 180°c (360°f) till they turn crisp.
+Cut into 2½“squares and keep aside.
+How to proceed
+Place a spoonful of the achari paneer mixture on a sheet of samosa pattis warqi and serve immediately.</t>
+  </si>
+  <si>
+    <t>achari dip recipe | healthy achar dip | Indian achari dip |</t>
+  </si>
+  <si>
+    <t>For Achar Dip
+3/4 cup hung curds (chakka dahi)
+salt to taste
+For The Achaari Mixture
+1/4 tsp fenugreek (methi) seeds
+1/4 tsp mustard seeds ( rai / sarson)
+1/2 tsp cumin seeds (jeera)
+1/2 tsp fennel seeds (saunf)
+1/4 tsp nigella seeds (kalonji)
+1/2 tsp oil
+a pinch of asafoetida (hing)
+1/4 cup chopped coriander (dhania)
+1/2 tsp finely chopped green chillies
+1/2 tbsp powdered sugar
+For Serving With Achar Dip
+khakhras</t>
+  </si>
+  <si>
+    <t>2 mins</t>
+  </si>
+  <si>
+    <t>1 mins</t>
+  </si>
+  <si>
+    <t>Method
+For the achaari mixture
+Heat the oil in a small non-stick pan, add the fenugreek seeds, mustard seeds, cumin seeds, fennel seeds and nigella seeds and sauté on a medium flame for 30 seconds.
+When the seeds crackle, add the asafoetida and mix well.
+Transfer the mixture into a deep bowl and allow the mixture to cool completely.
+Add the coriander, green chillies and powdered sugar and blend in a mixer to smooth paste using 2 tbsp of water. Keep aside.
+How to proceed to make achar dip
+To make achari dip, combine the achaari mixture, curds and salt in a deep bowl and mix well using a whisk.
+Refrigerate for at least 1 hour.
+Serve the achari dip chilled with khakhras.</t>
+  </si>
+  <si>
+    <t>Energy 28 cal
+Protein 0.9 g
+Carbohydrates 1.5 g
+Fiber 0 g
+Fat 1.5 g
+Cholesterol 3.4 mg
+Sodium 4.3 mg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -403,43 +940,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="42.6328125" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="75">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pagination feature added to pcos
</commit_message>
<xml_diff>
--- a/src/test/resources/outPutData.xlsx
+++ b/src/test/resources/outPutData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayesh\IdeaProjects\Data_Scraping_Framework_Demo1\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1605FC-DC0B-44AB-8B0D-04A9214EED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910B8151-698A-4934-B7A5-0FF4A7FF6D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="157">
   <si>
     <t>Recipe Name</t>
   </si>
@@ -585,6 +585,602 @@
 Fat 1.5 g
 Cholesterol 3.4 mg
 Sodium 4.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/a-checkerboard-of-roses--flower-arrangements-37154r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/a-truly-delectable-bunch--flower-arrangements-37261r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/a-bun-dantly-creative--flower-arrangements-37167r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/aam-chana-achar-rajasthani-pickle-3904r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/aam-ka-achaar-mango-pickle-punjabi-achar-30931r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/aam-ke-pakode-mango-bhajiya-36291r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/aam-ki-katki-ka-muraba-3427r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/aam-ki-launji-3901r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/aam-lassi-slush-2848r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/abc-juice-apple-beet-carrot-juice-6201r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achaari-aloo-roll--wraps-and-rolls-32665r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achaari-paneer-tikka-32939r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achaari-paneer-warqi-36293r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achar-dip-achari-dip-22718r</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achari-baingan-30888r</t>
+  </si>
+  <si>
+    <t>Achari Baingan</t>
+  </si>
+  <si>
+    <t>To Be Mixed Into A Marinade
+1 tbsp ginger-garlic (adrak-lehsun) paste
+1 tsp chilli powder
+1/2 tsp turmeric powder (haldi)
+salt to taste
+1 tsp oil
+Other Ingredients
+2 cups brinjals (baingan / eggplant) , cut into 1" cubes
+oil for deep frying
+1 tsp fennel seeds (saunf)
+1 tsp mustard seeds ( rai / sarson)
+1 tsp fenugreek (methi) seeds
+1 tsp nigella seeds (kalonji)
+1/2 tsp cumin seeds (jeera)
+1/2 tsp asafoetida (hing)
+2 tbsp oil
+1/2 cup sliced onions
+1 tsp ginger-garlic (adrak-lehsun) paste
+1 tsp chopped green chillies
+1/2 tsp turmeric powder (haldi)
+1/2 tsp chilli powder
+1/2 tsp punjabi garam masala
+1/2 tsp dried mango powder (amchur)
+salt to taste
+3/4 cup whisked curds (dahi)
+1/2 cup fresh cream
+For The Garnish
+2 tbsp finely chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>Method
+Combine the brinjals with the prepared marinade in a deep bowl and toss gently. Keep aside for 5 minutes.
+Heat the oil in a kadhai and deep-fry the marinade brinjals in it till they are golden brown in colour from all the sides.
+Drain on an absorbent paper and keep aside.
+Combine the fennel seeds, mustard seeds, fenugreek seeds, onion seeds, cumin seeds and asafoetida in a small bowl and keep aside.
+Heat the oil in a deep pan and add the above mixture.
+When the seeds crackle, add the onions, ginger-garlic paste and green chillies and sauté on a medium flame for 2 minutes.
+Add the turmeric powder, chilli powder, punjabi garam masala, dry mango powder and salt and sauté on a medium flame for 2 minutes.
+Add the curds, fried brinjals and fresh cream, mix gently and cook on a slow flame for 2 to 3 minutes, while stirring continuously.
+Serve hot garnished with coriander.</t>
+  </si>
+  <si>
+    <t>Energy 215 cal
+Protein 3.1 g
+Carbohydrates 6 g
+Fiber 4 g
+Fat 19.2 g
+Cholesterol 6 mg
+Sodium 18 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achari-dahi-bhindi-punjabi--sabji-22779r</t>
+  </si>
+  <si>
+    <t>achari dahi bhindi recipe | Punjabi dahi bhindi sabji | achari dahi wali bhindi | okra in achari curd gravy |</t>
+  </si>
+  <si>
+    <t>For Achari Dahi Bhindi
+4 cups sliced ladies finger (bhindi)
+5 tbsp oil
+2 tsp fennel seeds (saunf)
+2 tsp mustard seeds ( rai / sarson)
+1/2 tsp nigella seeds (kalonji)
+1/4 tsp fenugreek (methi) seeds
+1/4 tsp asafoetida (hing)
+2 tsp finely chopped ginger (adrak)
+3/4 cup chopped tomatoes
+salt to taste
+To Be Mixed Into A Curd Mixture
+1/2 cup whisked curds (dahi)
+1 tsp chilli powder
+1/4 tsp turmeric powder (haldi)
+2 tsp coriander-cumin seeds (dhania-jeera) powder
+salt to taste
+For Serving With Achari Dahi Bhindi
+rotis/parathas</t>
+  </si>
+  <si>
+    <t>13 mins</t>
+  </si>
+  <si>
+    <t>Method
+To make achari dahi bhindi, heat 4 tbsp of oil in a broad non-stick pan, add the ladies finger, mix gently and cook on a medium flame for 5 to 6 minutes, while tossing occasionally. Remove in a deep bowl and keep aside.
+Heat the remaining 1 tbsp of oil in the same broad non-stick pan, add the fennel seeds, mustard seeds, nigella seeds, fenugreek seeds and asafoetida and sauté on a medium flame for a few seconds.
+Add the ginger and sauté on a medium flame for 30 more seconds.
+Add the tomatoes, mix well and cook on a medium flame for 2 to 3 minutes, while stirring occasionally.
+Lower the flame, add the curd mixture, mix well and cook for 1 minute, while stirring continuously.
+Add the shallow-fried ladies finger and salt, mix well and cook on a medium flame for 1 to 2 minutes, while stirring occasionally.
+Serve the achari dahi bhindi hot with rotis or parathas.</t>
+  </si>
+  <si>
+    <t>Energy 328 cal
+Protein 4.8 g
+Carbohydrates 13.3 g
+Fiber 6.4 g
+Fat 27.6 g
+Cholesterol 5.3 mg
+Sodium 22.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achari-paneer-1736r</t>
+  </si>
+  <si>
+    <t>achari paneer recipe | Punjabi achari paneer | restaurant style achari paneer | healthy achari paneer |</t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>For Achari Paneer
+1 cup paneer (cottage cheese) cubes
+1 tbsp oil
+1 tsp fennel seeds (saunf)
+1/4 tsp mustard seeds ( rai / sarson)
+1/4 tsp fenugreek (methi) seeds
+1 tsp nigella seeds (kalonji)
+1/2 tsp cumin seeds (jeera)
+1/2 tsp asafoetida (hing)
+1/2 cup thinly sliced onions
+1/2 tsp turmeric powder (haldi)
+1/2 tsp chilli powder
+1/2 tsp black salt (sanchal)
+3/4 cup whisked curds (dahi)
+1 tsp plain flour (maida)
+2 tbsp chopped coriander (dhania)
+salt to taste</t>
+  </si>
+  <si>
+    <t>Method
+For achari paneer
+To make achari paneer, heat the oil in a deep non-stick pan, add the fennel seeds, mustard seeds, fenugreek seeds, nigella seeds, cumin seeds and asafoetida and sauté on a medium flame for 1 minute.
+Add the onion and sauté on a medium flame for 2 minutes.
+Add the paneer, turmeric, chilli powder, black salt, mix well and cook on a medium flame for 1 minute, while stirring occasionally.
+Add the curds, plain flour, mix well and cook on a medium flame for 1 to 2 minutes, while stirring occasionally.
+Switch off the flame, add the coriander and salt and mix well.
+Serve the achari paneer hot with rice or rotis.</t>
+  </si>
+  <si>
+    <t>Energy 381 cal
+Protein 13.4 g
+Carbohydrates 12.8 g
+Fiber 0.2 g
+Fat 29 g
+Cholesterol 12 mg
+Sodium 16.8 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achari-paneer-pulao-paneer-tikka-rice-7555r</t>
+  </si>
+  <si>
+    <t>achari paneer pulao recipe | Indian paneer tikka pulao | paneer tikka rice | achari biryani |</t>
+  </si>
+  <si>
+    <t>For Achari Paneer
+1 1/4 cups paneer (cottage cheese) cubes
+1 tbsp oil
+1 tsp mustard seeds ( rai / sarson)
+1/2 tsp fenugreek (methi) seeds
+1 tsp cumin seeds (jeera)
+1 tsp nigella seeds (kalonji)
+1 tsp fennel seeds (saunf)
+1/4 tsp turmeric powder (haldi)
+1 tsp chilli powder
+1/2 cup whisked curds (dahi)
+1 tbsp readymade green chilli pickle
+salt to taste
+Other Ingredients For Achari Paneer Pulao
+3 cups cooked rice (chawal)
+1 tbsp oil
+1 to 2 cinnamon (dalchini) sticks
+2 cloves (laung / lavang)
+1/2 tsp caraway seeds (shahjeera)
+2 cardamoms (elaichi)
+salt to taste
+For The Garnish
+1 tbsp finely chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>Method
+For achari paneer
+Heat the oil in a kadhai, add the mustard seeds, fenugreek seeds, cumin seeds, nigella seeds and fennel seeds.
+When the seeds crackle, add the turmeric powder, chilli powder and switch off the flame.
+Add the curds and mix well.
+Add the green chilli pickle and salt and mix well.
+Add the paneer cubes, mix gently and keep aside to marinate for 30 minutes.
+How to proceed
+To make the achari paneer pulao, heat the oil in a non-stick pan, add the cinnamon, cloves, caraway seeds and cardamom.
+When the caraway seeds crackle, add the rice and salt, mix well and cook on medium flame for 1 minute, while stirring continuously.
+Add the marinated paneer, mix well and cook on a medium flame for 1 to 2 minutes, while stirring occasionally.
+Serve the achari paneer pulao hot garnished with coriander.</t>
+  </si>
+  <si>
+    <t>Energy 377 cal
+Protein 10.1 g
+Carbohydrates 38.5 g
+Fiber 0.1 g
+Fat 19.7 g
+Cholesterol 4 mg
+Sodium 7.8 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/achari-paneer-tikka-4772r</t>
+  </si>
+  <si>
+    <t>achari paneer tikka recipe | Punjabi achari paneer tikka | achari paneer tikka on tawa | healthy achari paneer tikka |</t>
+  </si>
+  <si>
+    <t>For The Achari Marinade
+1 tbsp green chilli pickle
+1/2 cup hung curds (chakka dahi)
+1 tsp chopped garlic (lehsun)
+1 tsp fennel seeds (saunf)
+1/2 tsp mustard seeds ( rai / sarson)
+1/4 tsp fenugreek (methi) seeds
+1/4 tsp nigella seeds (kalonji)
+1 tsp cumin seeds (jeera)
+1/4 tsp turmeric powder (haldi)
+1 tbsp mustard (rai / sarson) oil
+salt to taste
+Other Ingredients For Achari Paneer Tikka
+1 1/2 cups paneer (cottage cheese) cubes
+oil for greasing and cooking</t>
+  </si>
+  <si>
+    <t>Method
+For the achari marinade
+Combine all the ingredients, except the curds in a mixer and blend to a coarse mixture.
+Transfer the mixture into a deep bowl, add the curds and mix well.
+How to proceed to make achari paneer tikka
+Add the paneer to the prepared achari marinade, mix gently and keep aside to marinate for 20 minutes.
+Arrange the marinated paneer cubes equally on satay sticks and keep aside.
+Heat a non-stick tava (griddle), grease it with little oil, place a few satays on it and cook on a medium flame, using a little oil, till they turn golden brown in colour from all the sides.
+Repeat step 3 to cook more satays.
+Serve the achari paneer tikka immediately.</t>
+  </si>
+  <si>
+    <t>Energy 295 cal
+Protein 9.4 g
+Carbohydrates 6.8 g
+Fiber 0 g
+Fat 24.4 g
+Cholesterol 8 mg
+Sodium 9.5 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/adai--diabetic-adai-recipe-22270r</t>
+  </si>
+  <si>
+    <t>healthy adai recipe | diabetic adai | Indian style dalia adai without rice | Indian snack for diabetes |</t>
+  </si>
+  <si>
+    <t>breakfast</t>
+  </si>
+  <si>
+    <t>For Adai
+1/2 cup broken wheat (dalia)
+1/4 cup green moong dal (split green gram)
+2 tbsp masoor (split red lentil) dal
+2 tbsp urad dal (split black lentils)
+1 tsp fenugreek (methi) seeds
+1/4 cup finely chopped onions
+a pinch of asafoetida (hing)
+1 tsp ginger-green chilli paste
+2 tbsp finely chopped coriander (dhania)
+1/4 tsp turmeric powder (haldi)
+1 tbsp chopped curry leaves (kadi patta)
+salt to taste
+3 tsp oil for cooking</t>
+  </si>
+  <si>
+    <t>40 mins</t>
+  </si>
+  <si>
+    <t>Method
+Combine the broken wheat, green moong dal, masoor dal, urad dal and fenugreek seeds in a deep bowl and soak in enough water for 2 hours. Drain well.
+Blend them in a mixer along with approx. ¾ cup of water to a coarse mixture.
+Transfer the mixture into a deep bowl, add the onions, asafoetida, ginger-green chilli paste, coriander, turmeric powder, curry leaves and salt and mix well.
+Heat a non-stick tava (griddle), sprinkle a little water on it and wipe it off gently using a muslin cloth.
+Pour a ladleful of the batter on it and spread it in a circular motion to make a 125 mm. (5”) diameter thin circle.
+Smear 1/8 tsp of oil over it and along the edges and cook on a medium flame till the adai turns golden brown in colour from both the sides.
+Fold over to make a semi-circle.
+Repeat steps 4 to 7 to make 23 more adais. .
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 53 cal
+Protein 2.2 g
+Carbohydrates 8.3 g
+Fiber 0.8 g
+Fat 1.2 g
+Cholesterol 0 mg
+Sodium 2.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/adai-recipe-adai-dosa-breakfast-534r</t>
+  </si>
+  <si>
+    <t>Adai Recipe, Adai Dosa, Breakfast</t>
+  </si>
+  <si>
+    <t>For Adai Dosa
+1 cup par-boiled rice (ukda chawal)
+1/4 cup toovar (arhar) dal
+1/4 cup chana dal (split bengal gram)
+2 tbsp urad dal (split black lentils)
+1 tsp roughly chopped ginger (adrak)
+4 dry red chillies (pandi)
+4 black peppercorns (kalimirch)
+1/2 tsp cumin seeds (jeera)
+1/4 cup finely chopped onions
+1/4 tsp asafoetida (hing)
+1 tbsp chopped curry leaves (kadi patta)
+2 tbsp grated coconut
+salt to taste
+coconut oil or oil for cooking
+For Serving With Adai Dosa
+coconut chutney</t>
+  </si>
+  <si>
+    <t>Method
+For adai dosa
+To make adai dosas, combine the rice, dals, ginger, peppercorns and red chillies in enough water in a deep bowl and keep aside to soak for 2 hours. Drain the water.
+Blend the mixture in a mixer to a coarse mixture using approx. 1¼ cup of water.
+Transfer the mixture into a deep bowl, add the onions, grated coconut, curry leaves, cumin seeds, asafoetida and salt. Mix well.
+Heat a non-stick tava (griddle), sprinkle a little water on the tava (griddle) and wipe it off gently using a muslin cloth.
+Pour a ladleful of the batter on it and spread it in a circular motion to make a 175 mm. (7”) diameter thin circle.
+Smear a little coconut oil over it and along the edges and cook on a medium flame till the adai dosa turns golden brown in colour and crisp.
+Turn over and cook on the other side as well.
+Fold over to make a semi-circle.
+Repeat with the remaining batter to make 9 more adai dosas.
+Serve the adai dosa immediately with coconut chutney.</t>
+  </si>
+  <si>
+    <t>Energy 114 cal
+Protein 3.8 g
+Carbohydrates 21.7 g
+Fiber 1.8 g
+Fat 1.4 g
+Cholesterol 0 mg
+Sodium 6.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/adai-protein-rich-adai-recipe-33240r</t>
+  </si>
+  <si>
+    <t>Adai, Protein Rich Adai Recipe</t>
+  </si>
+  <si>
+    <t>1/2 cup raw rice (chawal)
+1/4 cup toovar (arhar) dal
+1/4 cup chana dal (split bengal gram)
+1/4 cup urad dal (split black lentils)
+5 to 6 whole dry kashmiri red chillies , broken into pieces
+a pinch of asafoetida (hing)
+2 tbsp freshly grated coconut
+1/4 cup grated carrot
+1/4 cup finely chopped cabbage
+1/2 cup finely chopped onions
+1/4 cup finely chopped coriander (dhania)
+1 tbsp finely chopped curry leaves (kadi patta)
+salt to taste
+3 3/4 tsp oil for cooking</t>
+  </si>
+  <si>
+    <t>Method
+Clean, wash and soak the rice, dals and dry red chillies in enough water for 2 hours.
+Drain and blend in a mixer to a coarse paste using approx. 1¼ cups of water.
+Transfer the mixture into a deep bowl, add all the remaining ingredients and mix well.
+Heat a non-stick tava (griddle), sprinkle a little water on the tava (griddle) and wipe it off gently using a muslin cloth.
+Pour a ladleful of the batter on it and spread it in a circular motion to make a 175 mm. (7”) diameter thin circle.
+Smear ¼ tsp of oil over it and along the edges and cook on a medium flame till the adai turns golden brown in colour and crisp.
+Turnover and cook on another side as well.
+Fold over to make a semi-circle.
+Repeat with the remaining batter to make 14 more adais.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 73 cal
+Protein 2.7 g
+Carbohydrates 10.7 g
+Fiber 1.7 g
+Fat 2.2 g
+Cholesterol 0 mg
+Sodium 6.5 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/adrak-aur-ganne-ka-slush-sugarcane-and-ginger-slush-2850r</t>
+  </si>
+  <si>
+    <t>Adrak Aur Ganne ka Slush, Sugarcane and Ginger Slush</t>
+  </si>
+  <si>
+    <t>1 tbsp ginger (adrak) juice
+5 cups sugarcane juice
+1/2 cup powdered sugar
+1/2 tbsp lemon juice
+1/2 tsp salt</t>
+  </si>
+  <si>
+    <t>Method
+Combine all the ingredients in a deep bowl and mix well.
+Pour the mixture into a shallow aluminium container and freeze for 5 hours.
+Blend in a mixer till slushy and serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 115 cal
+Protein 0.2 g
+Carbohydrates 27.5 g
+Fiber 0 g
+Fat 0.4 g
+Cholesterol 0 mg
+Sodium 258.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/affogato-4752r</t>
+  </si>
+  <si>
+    <t>Affogato</t>
+  </si>
+  <si>
+    <t>2 scoops vanilla ice-cream
+1 1/2 tsp instant coffee powder
+1 tsp brandy
+1 tsp sugar
+For The Garnish
+1/2 tsp cinnamon (dalchini) powder</t>
+  </si>
+  <si>
+    <t>Method
+Boil the ¼ cup of water in a non-stick pan, add the coffee and sugar and mix well.
+Add the brandy and mix well.
+Place a scoop of ice-cream in each coffee mug and pour half the coffee mixture over each mug.
+Serve immediately garnished with the cinnamon powder.</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/afghani-paneer-30939r</t>
+  </si>
+  <si>
+    <t>Afghani Paneer</t>
+  </si>
+  <si>
+    <t>For Afghani Paneer
+2 cups paneer (cottage cheese) cubes
+To Be Ground Into A Smooth Powder
+1 tbsp melon seeds (charmagaz)
+3 tbsp cashew nuts (kaju)
+1 tbsp poppy seeds (khus-khus)
+To Be Mixed Into A Marinade
+1/4 cup fresh cream
+2 tbsp milk
+2 tbsp butter
+1 tsp white pepper powder
+1 tsp garam masala
+1 tsp green chilli paste
+salt to taste
+Other Ingredients For Afghani Paneer
+oil for greasing and cooking</t>
+  </si>
+  <si>
+    <t>Method
+Combine the paneer, prepared powder and prepared marinade in a deep bowl and mix gently.
+Keep aside for 2 hours.
+Thread 6 pieces of the marinaded paneer in each satay stick or a skewer.
+Heat a non-stick tava(griddle), grease it with little oil, place 4 marinated paneer satays on it and cook using a little oil on a medium flame for approx. 10 minutes or till they turn brown in colour from all the sides.
+Repeat steps 3 and 4 to make 4 more satays.
+Serve immediately.</t>
+  </si>
+  <si>
+    <t>Energy 219 cal
+Protein 5.9 g
+Carbohydrates 4 g
+Fiber 0.1 g
+Fat 19.9 g
+Cholesterol 8.1 mg
+Sodium 28.1 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/air-fried-bhindi-healthy-air-fryer-crispy-okra-42874r</t>
+  </si>
+  <si>
+    <t>air fried bhindi recipe | healthy air fryer crispy okra (ladies finger) | quick Indian air fried bhindi |</t>
+  </si>
+  <si>
+    <t>For Air Fried Bhindi
+3 cups ladies finger (bhindi)
+1/2 tsp olive oil
+To Be Mixed Into A Masala Powder
+1/2 tsp chaat masala
+1/4 tsp chilli powder
+1/4 tsp salt</t>
+  </si>
+  <si>
+    <t>Method
+For air fried bhindi
+To make air fried bhindi, wash the ladies finger, trim the tips from both the sides and discard them.
+Slice each bhindi into 4 pieces length wise, add olive oil and mix well.
+Place the bhindi in an air fryer and cook at 200°c for 10 minutes, while stirring once after 5 minutes.
+Add the masala powder and mix well.
+Serve healthy air fryer crispy okra (ladies finger) immediately.</t>
+  </si>
+  <si>
+    <t>Energy 43 cal
+Protein 1.9 g
+Carbohydrates 6.3 g
+Fiber 3.6 g
+Fat 1.2 g
+Cholesterol 0 mg
+Sodium 394.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/air-fried-shakarkand-indian-style-sweet-potato-fries-42873r</t>
+  </si>
+  <si>
+    <t>air fried shakarkand recipe | air fryer sweet potatoes | Indian style air fried sweet potatoes fries | quick air fryer sweet potatoes |</t>
+  </si>
+  <si>
+    <t>For Air Fried Shakarkand
+2 large sweet potato (shakarkand)
+1/2 tsp chaat masala
+1/4 tsp chilli powder
+1/8 tsp freshly ground black pepper (kalimirch)
+1/4 tsp salt
+1 1/2 tsp olive oil</t>
+  </si>
+  <si>
+    <t>14 mins</t>
+  </si>
+  <si>
+    <t>Method
+For air fried shakarkand
+To make the masala for air fried shakarkand ( sweet potatoes) in a small bowl put the chaat masala. Then add chilli powder, black pepper and salt. Mix well.
+Peel the shakarkand. Then cut into strips and cubes. We have cut into 2 different shapes to show you. You can use any shape.
+Brush the shakarkand with 1 tsp olive oil.
+Place the shakarkand in an air fryer and cook at 200 c for 14 minutes. At 5 minutes and 10 minutes, open the air fryer and toss the shakarkand each time and then continue cooking.
+Place the air fried shakarkand in a bowl. Add 1/2 tsp olive oil and toss.
+Add the masala powder and mix well.
+Serve air fried shakarkand immediately as it will remain crisp for a short while.</t>
+  </si>
+  <si>
+    <t>Energy 159 cal
+Protein 1.4 g
+Carbohydrates 33.1 g
+Fiber 4.6 g
+Fat 2.4 g
+Cholesterol 0 mg
+Sodium 204.4 mg</t>
   </si>
 </sst>
 </file>
@@ -940,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -951,12 +1547,12 @@
     <col min="2" max="3" bestFit="true" customWidth="true" width="42.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="75">
+    <row r="1" spans="1:11" ht="62.5">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -984,9 +1580,12 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1003,10 +1602,19 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="I2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -1020,10 +1628,16 @@
       <c r="H3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="J3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -1037,10 +1651,22 @@
       <c r="H4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="I4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -1057,10 +1683,16 @@
       <c r="I5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="J5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -1077,10 +1709,16 @@
       <c r="I6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="J6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
@@ -1097,10 +1735,19 @@
       <c r="I7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="J7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
       </c>
       <c r="E8" t="s">
         <v>39</v>
@@ -1117,10 +1764,19 @@
       <c r="I8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="J8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
       </c>
       <c r="E9" t="s">
         <v>45</v>
@@ -1137,10 +1793,16 @@
       <c r="I9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="J9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>
@@ -1157,10 +1819,16 @@
       <c r="I10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="J10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -1180,10 +1848,16 @@
       <c r="I11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
         <v>59</v>
@@ -1197,10 +1871,16 @@
       <c r="H12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="J12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>62</v>
@@ -1217,10 +1897,16 @@
       <c r="I13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="J13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>66</v>
@@ -1234,8 +1920,20 @@
       <c r="H14" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="I14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
       <c r="E15" t="s">
         <v>69</v>
       </c>
@@ -1250,6 +1948,353 @@
       </c>
       <c r="I15" t="s">
         <v>73</v>
+      </c>
+      <c r="J15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" t="s">
+        <v>104</v>
+      </c>
+      <c r="J19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" t="s">
+        <v>120</v>
+      </c>
+      <c r="I22" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>125</v>
+      </c>
+      <c r="I23" t="s">
+        <v>126</v>
+      </c>
+      <c r="J23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" t="s">
+        <v>130</v>
+      </c>
+      <c r="I24" t="s">
+        <v>131</v>
+      </c>
+      <c r="J24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" t="s">
+        <v>135</v>
+      </c>
+      <c r="I25" t="s">
+        <v>136</v>
+      </c>
+      <c r="J25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" t="s">
+        <v>140</v>
+      </c>
+      <c r="J26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" t="s">
+        <v>145</v>
+      </c>
+      <c r="J27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E28" t="s">
+        <v>148</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I28" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" t="s">
+        <v>153</v>
+      </c>
+      <c r="F29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" t="s">
+        <v>154</v>
+      </c>
+      <c r="H29" t="s">
+        <v>155</v>
+      </c>
+      <c r="I29" t="s">
+        <v>156</v>
+      </c>
+      <c r="J29" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>